<commit_message>
Revert "Merge branch 'ZamoraAngelo' into dev"
This reverts commit c4f32b97ac36eb7c6b7326ab1351bb7b66b5e9d5.
</commit_message>
<xml_diff>
--- a/LineaBase/ECI/LineaBase2/Gestion/ECI-CP.xlsx
+++ b/LineaBase/ECI/LineaBase2/Gestion/ECI-CP.xlsx
@@ -473,6 +473,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -480,7 +481,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,7 +699,7 @@
   <dimension ref="A1:H975"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -715,24 +715,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="29"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -1095,7 +1095,7 @@
       <c r="G22" s="21">
         <v>44409</v>
       </c>
-      <c r="H22" s="30">
+      <c r="H22" s="27">
         <v>1</v>
       </c>
     </row>
@@ -1116,7 +1116,7 @@
       <c r="G23" s="21">
         <v>44410</v>
       </c>
-      <c r="H23" s="30">
+      <c r="H23" s="27">
         <v>1</v>
       </c>
     </row>
@@ -1154,9 +1154,7 @@
       <c r="G25" s="21">
         <v>44422</v>
       </c>
-      <c r="H25" s="30">
-        <v>0.5</v>
-      </c>
+      <c r="H25" s="27"/>
     </row>
     <row r="26" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
@@ -1177,9 +1175,7 @@
       <c r="G26" s="21">
         <v>44436</v>
       </c>
-      <c r="H26" s="30">
-        <v>0.3</v>
-      </c>
+      <c r="H26" s="27"/>
     </row>
     <row r="27" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
@@ -1203,9 +1199,7 @@
       <c r="G27" s="21">
         <v>44439</v>
       </c>
-      <c r="H27" s="30">
-        <v>0.4</v>
-      </c>
+      <c r="H27" s="27"/>
     </row>
     <row r="28" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
@@ -1229,9 +1223,7 @@
       <c r="G28" s="21">
         <v>44442</v>
       </c>
-      <c r="H28" s="30">
-        <v>0.4</v>
-      </c>
+      <c r="H28" s="27"/>
     </row>
     <row r="29" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">

</xml_diff>